<commit_message>
Base version of backtesting project by GShah
</commit_message>
<xml_diff>
--- a/Input_files/Strategies.xlsx
+++ b/Input_files/Strategies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PycharmProjects\Backtesting\Input_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6CC15A0-F8E8-4294-91F6-8719C263A16D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81BAFA2F-59B2-42AF-8695-C51E0C00231B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{1EEBE60A-616E-43E0-89E0-E42973C85DA2}"/>
   </bookViews>
@@ -75,9 +75,6 @@
     <t>sma_crossover_system</t>
   </si>
   <si>
-    <t>wma20_system</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
@@ -85,6 +82,9 @@
   </si>
   <si>
     <t>roc_system</t>
+  </si>
+  <si>
+    <t>wma20_macd_system</t>
   </si>
 </sst>
 </file>
@@ -445,7 +445,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,7 +502,7 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3">
         <v>20</v>
@@ -510,10 +510,10 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
         <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
       </c>
       <c r="C4">
         <v>20</v>
@@ -521,7 +521,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5">
         <v>30</v>

</xml_diff>